<commit_message>
Creación de ruta para la carga de archivos
</commit_message>
<xml_diff>
--- a/uploads/plantillas/vehiculos.xlsx
+++ b/uploads/plantillas/vehiculos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IngnovaOtt\SuperTransporte\POLIZA\backend_poliza\uploads\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{955DAE61-AF5D-4A47-9A4E-325C45EAA70F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E60FBE-755B-472B-A17A-C9108E78D340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5355" yWindow="3255" windowWidth="21600" windowHeight="11235" xr2:uid="{7028A36A-A99D-40EB-8645-249C7FA73674}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7028A36A-A99D-40EB-8645-249C7FA73674}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,21 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>PLACA</t>
-  </si>
-  <si>
-    <t>MARCA</t>
-  </si>
-  <si>
-    <t>MODELO</t>
-  </si>
-  <si>
-    <t>TIPO O SERVICIO</t>
-  </si>
-  <si>
-    <t>CLASE DE SERVICIO</t>
   </si>
   <si>
     <t>CANTIDAD DE PASAJEROS</t>
@@ -97,7 +85,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,45 +420,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806917B6-05B5-4172-8BE2-91184BE0B079}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Actualizacion de usuarios y creacion de estados
</commit_message>
<xml_diff>
--- a/uploads/plantillas/vehiculos.xlsx
+++ b/uploads/plantillas/vehiculos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IngnovaOtt\SuperTransporte\POLIZA\backend_poliza\uploads\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E60FBE-755B-472B-A17A-C9108E78D340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5DF9EE-5A38-4DC8-8B3A-2491BE843783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7028A36A-A99D-40EB-8645-249C7FA73674}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,13 +62,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,9 +97,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,21 +438,21 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>